<commit_message>
Update financial DB download file
</commit_message>
<xml_diff>
--- a/static/download/xls/ANSP_Financial_Data.xlsx
+++ b/static/download/xls/ANSP_Financial_Data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -8,11 +8,11 @@
   <sheets>
     <sheet name="Copyright notice and disclaimer" sheetId="6" state="visible" r:id="rId1"/>
     <sheet name="META" sheetId="17" state="visible" r:id="rId2"/>
-    <sheet name="2017" sheetId="28" state="visible" r:id="rId3"/>
-    <sheet name="2018" sheetId="29" state="visible" r:id="rId4"/>
-    <sheet name="2019" sheetId="30" state="visible" r:id="rId5"/>
-    <sheet name="2020" sheetId="31" state="visible" r:id="rId6"/>
-    <sheet name="2021" sheetId="32" state="visible" r:id="rId7"/>
+    <sheet name="2017" sheetId="38" state="visible" r:id="rId3"/>
+    <sheet name="2018" sheetId="39" state="visible" r:id="rId4"/>
+    <sheet name="2019" sheetId="40" state="visible" r:id="rId5"/>
+    <sheet name="2020" sheetId="41" state="visible" r:id="rId6"/>
+    <sheet name="2021" sheetId="42" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="3">
     <font>
@@ -961,7 +961,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -991,10 +991,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="false" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1020,10 +1020,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -4130,10 +4130,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -7240,10 +7240,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -10350,10 +10350,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -13460,10 +13460,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -13730,85 +13730,85 @@
         <v>2021</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="D4" t="n">
-        <v>10.1465</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>147</v>
       </c>
       <c r="F4" t="n">
-        <v>2410</v>
+        <v>162.256</v>
       </c>
       <c r="G4" t="n">
-        <v>-2194</v>
+        <v>-144.513</v>
       </c>
       <c r="H4" t="n">
-        <v>216</v>
+        <v>17.743</v>
       </c>
       <c r="I4" t="n">
-        <v>-192</v>
+        <v>-10.673</v>
       </c>
       <c r="J4" t="n">
-        <v>23.25</v>
+        <v>7.07</v>
       </c>
       <c r="K4" t="n">
-        <v>65</v>
+        <v>-1.378</v>
       </c>
       <c r="L4" t="n">
-        <v>88.25</v>
+        <v>11.379</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>5991</v>
+        <v>141.487</v>
       </c>
       <c r="O4" t="n">
-        <v>4924</v>
+        <v>275.802</v>
       </c>
       <c r="P4" t="n">
-        <v>10915</v>
+        <v>417.289</v>
       </c>
       <c r="Q4" t="n">
-        <v>677</v>
+        <v>260.405</v>
       </c>
       <c r="R4" t="n">
-        <v>1028</v>
+        <v>39.442</v>
       </c>
       <c r="S4" t="n">
-        <v>9209</v>
+        <v>117.442</v>
       </c>
       <c r="T4" t="n">
-        <v>10237</v>
+        <v>156.884</v>
       </c>
       <c r="U4" t="n">
-        <v>4267</v>
+        <v>116.669</v>
       </c>
       <c r="V4" t="n">
-        <v>709.870100273473</v>
+        <v>294.673731774996</v>
       </c>
       <c r="W4" t="n">
-        <v>475</v>
+        <v>-23.654</v>
       </c>
       <c r="X4" t="n">
-        <v>-354</v>
+        <v>70.04</v>
       </c>
       <c r="Y4" t="n">
-        <v>-815</v>
+        <v>-0.898</v>
       </c>
       <c r="Z4" t="n">
-        <v>-693.25</v>
+        <v>45.488</v>
       </c>
       <c r="AA4" t="n">
-        <v>-354</v>
+        <v>-11.775</v>
       </c>
       <c r="AB4" t="n">
-        <v>121</v>
+        <v>-35.429</v>
       </c>
     </row>
     <row r="5">
@@ -13816,84 +13816,428 @@
         <v>2021</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="D5" t="n">
-        <v>1.0811</v>
+        <v>10.1465</v>
       </c>
       <c r="E5" t="s">
         <v>147</v>
       </c>
       <c r="F5" t="n">
+        <v>2410</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-2194</v>
+      </c>
+      <c r="H5" t="n">
+        <v>216</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-192</v>
+      </c>
+      <c r="J5" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="K5" t="n">
+        <v>65</v>
+      </c>
+      <c r="L5" t="n">
+        <v>88.25</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>5991</v>
+      </c>
+      <c r="O5" t="n">
+        <v>4924</v>
+      </c>
+      <c r="P5" t="n">
+        <v>10915</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>677</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1028</v>
+      </c>
+      <c r="S5" t="n">
+        <v>9209</v>
+      </c>
+      <c r="T5" t="n">
+        <v>10237</v>
+      </c>
+      <c r="U5" t="n">
+        <v>4267</v>
+      </c>
+      <c r="V5" t="n">
+        <v>709.870100273473</v>
+      </c>
+      <c r="W5" t="n">
+        <v>475</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-354</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>-815</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>-693.25</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>-354</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" t="n">
+        <v>19.797503</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-19.003318</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.794185</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-3.906371</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-3.112186</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-0.04245</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-3.154636</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>31.848425</v>
+      </c>
+      <c r="O6" t="n">
+        <v>7.521389</v>
+      </c>
+      <c r="P6" t="n">
+        <v>39.369814</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>32.356607</v>
+      </c>
+      <c r="R6" t="n">
+        <v>4.322769</v>
+      </c>
+      <c r="S6" t="n">
+        <v>2.690438</v>
+      </c>
+      <c r="T6" t="n">
+        <v>7.013207</v>
+      </c>
+      <c r="U6" t="n">
+        <v>2.871421</v>
+      </c>
+      <c r="V6" t="n">
+        <v>55.1518774247739</v>
+      </c>
+      <c r="W6" t="n">
+        <v>-2.262872</v>
+      </c>
+      <c r="X6" t="n">
+        <v>-4.282818</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>-0.223366</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>-6.769056</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>-4.285703</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>-6.548575</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" t="n">
+        <v>7.437</v>
+      </c>
+      <c r="E7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" t="n">
+        <v>884.256</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-797.606</v>
+      </c>
+      <c r="H7" t="n">
+        <v>86.65</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-107.583</v>
+      </c>
+      <c r="J7" t="n">
+        <v>5.412</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-10.655</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-3.314</v>
+      </c>
+      <c r="M7" t="n">
+        <v>26.345</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1298.281</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1018.242</v>
+      </c>
+      <c r="P7" t="n">
+        <v>2316.523</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1082.781</v>
+      </c>
+      <c r="R7" t="n">
+        <v>337.249</v>
+      </c>
+      <c r="S7" t="n">
+        <v>896.493</v>
+      </c>
+      <c r="T7" t="n">
+        <v>1233.742</v>
+      </c>
+      <c r="U7" t="n">
+        <v>39.813</v>
+      </c>
+      <c r="V7" t="n">
+        <v>18.2192022126213</v>
+      </c>
+      <c r="W7" t="n">
+        <v>-286.908</v>
+      </c>
+      <c r="X7" t="n">
+        <v>-82.449</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>398.75</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>29.393</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>-82.449</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>-369.357</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" t="n">
+        <v>26.898</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-18.108</v>
+      </c>
+      <c r="H8" t="n">
+        <v>8.79</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-3.906</v>
+      </c>
+      <c r="J8" t="n">
+        <v>4.884</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-0.014</v>
+      </c>
+      <c r="L8" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>45.145</v>
+      </c>
+      <c r="O8" t="n">
+        <v>14.703</v>
+      </c>
+      <c r="P8" t="n">
+        <v>59.848</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>47.112</v>
+      </c>
+      <c r="R8" t="n">
+        <v>5.268</v>
+      </c>
+      <c r="S8" t="n">
+        <v>7.468</v>
+      </c>
+      <c r="T8" t="n">
+        <v>12.736</v>
+      </c>
+      <c r="U8" t="n">
+        <v>6.914</v>
+      </c>
+      <c r="V8" t="n">
+        <v>139.364369339518</v>
+      </c>
+      <c r="W8" t="n">
+        <v>-0.491</v>
+      </c>
+      <c r="X8" t="n">
+        <v>-3.239</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>-1.431</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>-5.161</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>-2.262</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>-2.753</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.0811</v>
+      </c>
+      <c r="E9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F9" t="n">
         <v>348.817</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G9" t="n">
         <v>-401.016</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H9" t="n">
         <v>-52.199</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I9" t="n">
         <v>-62.82</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J9" t="n">
         <v>-112.947</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K9" t="n">
         <v>-6.574</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L9" t="n">
         <v>-119.408</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M9" t="n">
         <v>2.072</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N9" t="n">
         <v>378.656</v>
       </c>
-      <c r="O5" t="n">
+      <c r="O9" t="n">
         <v>180.596</v>
       </c>
-      <c r="P5" t="n">
+      <c r="P9" t="n">
         <v>559.252</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="Q9" t="n">
         <v>186.525</v>
       </c>
-      <c r="R5" t="n">
+      <c r="R9" t="n">
         <v>112.363</v>
       </c>
-      <c r="S5" t="n">
+      <c r="S9" t="n">
         <v>260.365</v>
       </c>
-      <c r="T5" t="n">
+      <c r="T9" t="n">
         <v>372.728</v>
       </c>
-      <c r="U5" t="n">
+      <c r="U9" t="n">
         <v>102.142</v>
       </c>
-      <c r="V5" t="n">
+      <c r="V9" t="n">
         <v>92.9684351746564</v>
       </c>
-      <c r="W5" t="n">
+      <c r="W9" t="n">
         <v>-50.2</v>
       </c>
-      <c r="X5" t="n">
+      <c r="X9" t="n">
         <v>-33.88</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="Y9" t="n">
         <v>50.93</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="Z9" t="n">
         <v>-33.15</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AA9" t="n">
         <v>-35.387</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AB9" t="n">
         <v>-85.587</v>
       </c>
     </row>

</xml_diff>